<commit_message>
Update Whey Protein's Price
</commit_message>
<xml_diff>
--- a/Plan to use MBO.xlsx
+++ b/Plan to use MBO.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\96_Personal_Items\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18765" windowHeight="7260"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -284,7 +279,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -319,7 +314,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -496,7 +491,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -507,7 +502,7 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,7 +531,7 @@
       </c>
       <c r="B2" s="2">
         <f>SUMIF(D:D,$D$4,H:H)</f>
-        <v>10150000</v>
+        <v>10030000</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -545,7 +540,7 @@
       </c>
       <c r="B3" s="2">
         <f>B1-B2</f>
-        <v>3850000</v>
+        <v>3970000</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>20</v>
@@ -784,11 +779,11 @@
         <v>42</v>
       </c>
       <c r="G20" s="2">
-        <v>1350000</v>
+        <v>1230000</v>
       </c>
       <c r="H20" s="2">
         <f t="shared" si="0"/>
-        <v>1350000</v>
+        <v>1230000</v>
       </c>
     </row>
     <row r="21" spans="4:8" x14ac:dyDescent="0.25">

</xml_diff>